<commit_message>
Tried other backgrounds using shapes
</commit_message>
<xml_diff>
--- a/ColumnChartFormatting.xlsx
+++ b/ColumnChartFormatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{24E00A83-CC1D-44F8-AEFB-2F12B4B8500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F686E36-0CC5-4AAF-928C-48FA8C5B872D}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{24E00A83-CC1D-44F8-AEFB-2F12B4B8500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E40B7276-9334-4B1B-A7DE-F20364CB093D}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1011,7 +1011,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{6178EE97-2451-4C98-98AE-4FB246CFFED3}" type="CELLRANGE">
+                    <a:fld id="{FD5469EC-0C5B-407A-B6FE-F64B6238EAC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1000" b="1">
@@ -1077,7 +1077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B5B1D50-AF36-479E-948B-64DE3425E70E}" type="CELLRANGE">
+                    <a:fld id="{40E281A7-DE98-4DA1-9642-C532373F73FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1111,7 +1111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E9522AA-E265-411E-A57B-A37EBE62FFCE}" type="CELLRANGE">
+                    <a:fld id="{929E29C6-2A32-43DD-ADC2-BD02B8DFD21D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1145,7 +1145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58462C06-E120-495E-9CCF-3DE233C41092}" type="CELLRANGE">
+                    <a:fld id="{79753B8E-92E9-4F97-93D4-342EA8D97B89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1323,7 +1323,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{BB13B94A-7F40-4600-A328-EF68DE5F6F1E}" type="CELLRANGE">
+                    <a:fld id="{0A9198F8-6E6D-49F4-BAFA-2BBCFEB2ABF3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr b="1">
@@ -1389,7 +1389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B2B37CE-131C-4865-9A9F-39AF8FECB80D}" type="CELLRANGE">
+                    <a:fld id="{D6225931-C2F2-4E03-918F-8D26E315B340}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1423,7 +1423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B56A4D33-175D-485C-84CC-AC4A58B2BB61}" type="CELLRANGE">
+                    <a:fld id="{17797DC9-2E02-4224-AF8A-54AC202FED2F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1731,25 +1731,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="bg1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="shape">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -2365,42 +2347,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4024A33-BC8E-33B4-C271-2EA0CD27FDB5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
@@ -2428,7 +2374,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2447,93 +2393,218 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>554354</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>327659</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="Group 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75F8DE54-1CFA-1AB4-CC97-BA9B95DB8CA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2905E4EE-56BE-CE19-410B-393014BC240C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4370070" y="1221105"/>
-          <a:ext cx="3905250" cy="462915"/>
+          <a:off x="4208144" y="941070"/>
+          <a:ext cx="4650105" cy="3507105"/>
+          <a:chOff x="4170044" y="1078230"/>
+          <a:chExt cx="4650105" cy="3514725"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="8" name="Group 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290CE332-C784-5F32-62D3-8B6AC7F00291}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="4173854" y="1082040"/>
+            <a:ext cx="4650105" cy="3507105"/>
+            <a:chOff x="4170044" y="1120140"/>
+            <a:chExt cx="4657725" cy="3528060"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Rectangle 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E72DCCC-9D81-B62F-8699-C2F2FAF9EA4B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4170044" y="1120140"/>
+              <a:ext cx="4648200" cy="3528060"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="1000">
+                  <a:schemeClr val="bg1"/>
+                </a:gs>
+                <a:gs pos="91000">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:path path="circle">
+                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+              </a:path>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4024A33-BC8E-33B4-C271-2EA0CD27FDB5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="4267199" y="1200150"/>
+            <a:ext cx="4560570" cy="2914650"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="TextBox 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75F8DE54-1CFA-1AB4-CC97-BA9B95DB8CA9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4368165" y="1217295"/>
+            <a:ext cx="3909060" cy="464820"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Sales in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Product A</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t> driving </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>North's Performance</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0"/>
-            <a:t>Regional</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> product sales</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Sales in </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Product A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t> driving </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>North's Performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>Regional</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+              <a:t> product sales</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2730,7 +2801,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
I have figured out how to do the gradient
</commit_message>
<xml_diff>
--- a/ColumnChartFormatting.xlsx
+++ b/ColumnChartFormatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{24E00A83-CC1D-44F8-AEFB-2F12B4B8500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E40B7276-9334-4B1B-A7DE-F20364CB093D}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{24E00A83-CC1D-44F8-AEFB-2F12B4B8500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB93D2F5-6DDA-447B-9162-DC81F8F54E2C}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -401,6 +401,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFE6E6E6"/>
+      <color rgb="FFD7D7D7"/>
       <color rgb="FFB6B4B6"/>
       <color rgb="FF4C8DCD"/>
     </mruColors>
@@ -1011,7 +1013,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{FD5469EC-0C5B-407A-B6FE-F64B6238EAC6}" type="CELLRANGE">
+                    <a:fld id="{D73F166A-11F2-464F-98B1-A5C3726DD3E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1000" b="1">
@@ -1077,7 +1079,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40E281A7-DE98-4DA1-9642-C532373F73FB}" type="CELLRANGE">
+                    <a:fld id="{B0022D59-98B4-4D58-8070-C7F1A64A5005}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1111,7 +1113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{929E29C6-2A32-43DD-ADC2-BD02B8DFD21D}" type="CELLRANGE">
+                    <a:fld id="{23C6F3C6-B375-4888-B0D5-6DA026DC1184}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1145,7 +1147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79753B8E-92E9-4F97-93D4-342EA8D97B89}" type="CELLRANGE">
+                    <a:fld id="{A428E1FD-47B1-4D15-ABAA-A18BAA008F9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1323,7 +1325,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{0A9198F8-6E6D-49F4-BAFA-2BBCFEB2ABF3}" type="CELLRANGE">
+                    <a:fld id="{E8D479E2-BD79-48B1-A947-9012B4762B39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr b="1">
@@ -1389,7 +1391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6225931-C2F2-4E03-918F-8D26E315B340}" type="CELLRANGE">
+                    <a:fld id="{F0A972E7-0B85-4E22-9B54-7227A48DA47B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1423,7 +1425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17797DC9-2E02-4224-AF8A-54AC202FED2F}" type="CELLRANGE">
+                    <a:fld id="{365DF2FC-FABD-45E0-A181-30EAF7FB5F82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2393,23 +2395,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>554354</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121903</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>327659</xdr:colOff>
+      <xdr:colOff>382905</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Group 8">
+        <xdr:cNvPr id="3" name="Group 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2905E4EE-56BE-CE19-410B-393014BC240C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32687B01-9740-9CE0-33B3-7E866291B402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2417,117 +2419,103 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4208144" y="941070"/>
-          <a:ext cx="4650105" cy="3507105"/>
-          <a:chOff x="4170044" y="1078230"/>
-          <a:chExt cx="4650105" cy="3514725"/>
+          <a:off x="4267200" y="809608"/>
+          <a:ext cx="4650105" cy="3476642"/>
+          <a:chOff x="4208144" y="899152"/>
+          <a:chExt cx="4650105" cy="3484262"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="8" name="Group 7">
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290CE332-C784-5F32-62D3-8B6AC7F00291}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E72DCCC-9D81-B62F-8699-C2F2FAF9EA4B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
           <a:xfrm>
-            <a:off x="4173854" y="1082040"/>
-            <a:ext cx="4650105" cy="3507105"/>
-            <a:chOff x="4170044" y="1120140"/>
-            <a:chExt cx="4657725" cy="3528060"/>
+            <a:off x="4208144" y="899152"/>
+            <a:ext cx="4648216" cy="3484262"/>
           </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="Rectangle 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E72DCCC-9D81-B62F-8699-C2F2FAF9EA4B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4170044" y="1120140"/>
-              <a:ext cx="4648200" cy="3528060"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="1000">
-                  <a:schemeClr val="bg1"/>
-                </a:gs>
-                <a:gs pos="91000">
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-              </a:path>
-              <a:tileRect/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Chart 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4024A33-BC8E-33B4-C271-2EA0CD27FDB5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="4267199" y="1200150"/>
-            <a:ext cx="4560570" cy="2914650"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </xdr:grpSp>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="89000">
+                <a:srgbClr val="D7D7D7">
+                  <a:alpha val="49804"/>
+                </a:srgbClr>
+              </a:gs>
+              <a:gs pos="41000">
+                <a:srgbClr val="E6E6E6"/>
+              </a:gs>
+            </a:gsLst>
+            <a:path path="circle">
+              <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            </a:path>
+            <a:tileRect/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="4" name="Chart 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4024A33-BC8E-33B4-C271-2EA0CD27FDB5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="4308950" y="1029906"/>
+          <a:ext cx="4549299" cy="2887578"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="7" name="TextBox 6">
@@ -2541,8 +2529,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4368165" y="1217295"/>
-            <a:ext cx="3909060" cy="464820"/>
+            <a:off x="4411980" y="1026400"/>
+            <a:ext cx="3914775" cy="460002"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2801,7 +2789,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>